<commit_message>
adjusted spacing on main form and added autoscroll and modal placement to try and make pages load towards the top instead of middle in wellbridge.com
</commit_message>
<xml_diff>
--- a/z_Documents/Online Enrollment Check List.xlsx
+++ b/z_Documents/Online Enrollment Check List.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>Email Contract</t>
   </si>
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,11 +1396,19 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="A5" s="3">
+        <v>45936</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
corrected error on payment pages and reporting of errors, removed autoscroll to top from contract page
</commit_message>
<xml_diff>
--- a/z_Documents/Online Enrollment Check List.xlsx
+++ b/z_Documents/Online Enrollment Check List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="6915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>Email Contract</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Phase 2</t>
   </si>
   <si>
-    <t>Contract - base on actual membership type</t>
-  </si>
-  <si>
     <t>Unlimited Childcare</t>
   </si>
   <si>
@@ -338,6 +335,12 @@
   </si>
   <si>
     <t>removed from inventory per John - I removed from web_addons</t>
+  </si>
+  <si>
+    <t>Contract Text - base on actual membership type</t>
+  </si>
+  <si>
+    <t>No Juniors for Any club</t>
   </si>
 </sst>
 </file>
@@ -1339,12 +1342,12 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1370,7 +1373,7 @@
         <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1407,10 +1410,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4"/>
-      <c r="C6" t="s">
+      <c r="A6" s="3">
+        <v>45936</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1429,28 +1439,40 @@
         <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>86</v>
+      <c r="A9" s="3">
+        <v>45929</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>45929</v>
+        <v>45943</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>88</v>
+      <c r="A11" s="3">
+        <v>45931</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1461,18 +1483,18 @@
         <v>77</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>45931</v>
+        <v>45933</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1483,23 +1505,23 @@
         <v>77</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>45933</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>45932</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="13" t="s">
-        <v>93</v>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1510,23 +1532,17 @@
         <v>77</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>45932</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="13" t="s">
-        <v>94</v>
+      <c r="C21" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,7 +1577,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.1.6 in production for final testing, adjusted some font sizes
</commit_message>
<xml_diff>
--- a/z_Documents/Online Enrollment Check List.xlsx
+++ b/z_Documents/Online Enrollment Check List.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
   <si>
     <t>Email Contract</t>
   </si>
@@ -341,13 +341,16 @@
   </si>
   <si>
     <t>No Juniors for Any club</t>
+  </si>
+  <si>
+    <t>Email Club GM and PT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +375,14 @@
     <font>
       <b/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -411,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -432,6 +443,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1339,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,20 +1520,17 @@
         <v>92</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="13" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>45932</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1532,55 +1541,67 @@
         <v>77</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>45932</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="13" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="13" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="14" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the cart scolling, except it doesn't stop before the footer
</commit_message>
<xml_diff>
--- a/z_Documents/Online Enrollment Check List.xlsx
+++ b/z_Documents/Online Enrollment Check List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="6915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="6915" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
   <si>
     <t>Email Contract</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>Email Club GM and PT</t>
+  </si>
+  <si>
+    <t>Adjust for Cell Phones</t>
   </si>
 </sst>
 </file>
@@ -1351,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,30 +1524,30 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="3">
+        <v>45951</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="13" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>45932</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45932</v>
       </c>
@@ -1552,51 +1555,65 @@
         <v>77</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>45932</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="13" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="14" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.1.9 re-corrected once again the amounts and taxes being entered into BOSS
</commit_message>
<xml_diff>
--- a/z_Documents/Online Enrollment Check List.xlsx
+++ b/z_Documents/Online Enrollment Check List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="6915" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15240" windowHeight="6915" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="108">
   <si>
     <t>Email Contract</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>Adjust for Cell Phones</t>
+  </si>
+  <si>
+    <t>Branded for Wellbridge</t>
   </si>
 </sst>
 </file>
@@ -1354,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,37 +1528,37 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>45951</v>
+        <v>45945</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>45951</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
-    </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="13" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>45932</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,54 +1569,65 @@
         <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45932</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="13" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="13" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="14" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>